<commit_message>
added code to makeTextures to compute grating position; added grating display to fix_and_grat.m; other neurotic tidying
</commit_message>
<xml_diff>
--- a/ST_SEQ/LOAD/texts.xlsx
+++ b/ST_SEQ/LOAD/texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magda/Documents/0_MEG/PRED_ATT/ST_SEQ/LOAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E5591F-EDD6-5941-8284-36E3EBACD2EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BBCC20-914B-DF41-8AD5-A6E5A32A3F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{7E3F9E06-4516-8741-A882-C7F13C0C2DD9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Welcome</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Presiona XXX dos veces para EMPEZAR la calibraciÃ³n o YYY para volver atrÃ¡s...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In this experiment you will need to keep your focus on the center of the fixation cross shown below. </t>
   </si>
   <si>
     <t>This is not always easy since you will be seeing four visual objects, known as gratings, like you will see on the following screen.</t>
@@ -388,13 +385,25 @@
   </si>
   <si>
     <t>Next Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this experiment you will need to keep your focus on the center of the fixation DOT shown below. </t>
+  </si>
+  <si>
+    <t>Welcome to the BCBL!! Let's get going!!!</t>
+  </si>
+  <si>
+    <t>In this experiment you will always need to keep your eyes on the center dot (shown below)</t>
+  </si>
+  <si>
+    <t>It''s not always easy to fixate the cross because there will be many ''gratings'' on screen. As you''re about to see now…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -444,6 +453,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA020F0"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -465,11 +480,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3579D91F-97A3-0840-A950-C2B8A3215C24}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A23"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -811,227 +827,227 @@
     </row>
     <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
@@ -1042,13 +1058,28 @@
     </row>
     <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B28" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B29" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B30" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added code to makeTextures to compute grating position; added grating display to fix_and_grat.m
</commit_message>
<xml_diff>
--- a/ST_SEQ/LOAD/texts.xlsx
+++ b/ST_SEQ/LOAD/texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magda/Documents/0_MEG/PRED_ATT/ST_SEQ/LOAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BBCC20-914B-DF41-8AD5-A6E5A32A3F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC0B754-E29E-9448-96F7-9B42AB9164EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{7E3F9E06-4516-8741-A882-C7F13C0C2DD9}"/>
   </bookViews>
@@ -396,7 +396,7 @@
     <t>In this experiment you will always need to keep your eyes on the center dot (shown below)</t>
   </si>
   <si>
-    <t>It''s not always easy to fixate the cross because there will be many ''gratings'' on screen. As you''re about to see now…</t>
+    <t>It's not always easy to fixate the cross because there will be four ''gratings'' on screen. As you're about to see now…</t>
   </si>
 </sst>
 </file>

</xml_diff>